<commit_message>
Performed the analysis using a decision tree model
</commit_message>
<xml_diff>
--- a/Feature_Dictionary.xlsx
+++ b/Feature_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abraham/Documents/Comp Sci Projects/Wayfair_ML_Challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCC16BA-33C5-684B-B1EA-E5CA2EDAD708}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44145EBA-7138-4A49-8DBC-BC372416F366}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -931,7 +931,7 @@
     <t>Nonempty. External Application, Internal Application, Internal Customer Scrape, Gateway, Social - Paid, Search - Paid, Other, Quotes, Affiliates, Referral, Bulk Upload, Email, Display - Retargeting, Display - Acquisition, Self ID, Partners. Ignore.</t>
   </si>
   <si>
-    <t>Nonempty. Active, Enrolled, In Progress, Unconfirmed. Convert</t>
+    <t>Nonempty. Primary, Purchaser, Other, None. Convert</t>
   </si>
   <si>
     <t>Nonempty. 1to2, 3to5, 6to10, 11to25, 25plus, None. Convert</t>
@@ -943,9 +943,6 @@
     <t>Nonempty. Convert</t>
   </si>
   <si>
-    <t>Nonempty. Primary, Purchaser, Other, None. Ignore</t>
-  </si>
-  <si>
     <t>Nonempty. 1, 2to5, 6to10, 11to50, 50plus, None. Convert and Revenue</t>
   </si>
   <si>
@@ -962,6 +959,9 @@
   </si>
   <si>
     <t>Calculated by: totalrev / (numbamorder + numselforder). Revenue</t>
+  </si>
+  <si>
+    <t>Nonempty. Active, Enrolled, In Progress, Unconfirmed, Inactive. Ignore since values differ for training and testing sets</t>
   </si>
 </sst>
 </file>
@@ -1469,8 +1469,8 @@
   <dimension ref="A1:D184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1561,7 +1561,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1617,7 +1617,7 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1631,7 +1631,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1673,7 +1673,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1687,7 +1687,7 @@
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1701,7 +1701,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1715,7 +1715,7 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1729,7 +1729,7 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1743,7 +1743,7 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1757,7 +1757,7 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1771,7 +1771,7 @@
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1785,7 +1785,7 @@
         <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1799,7 +1799,7 @@
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1813,7 +1813,7 @@
         <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1827,7 +1827,7 @@
         <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1841,7 +1841,7 @@
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1877,7 +1877,7 @@
         <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1891,7 +1891,7 @@
         <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1952,7 +1952,7 @@
         <v>67</v>
       </c>
       <c r="D35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1966,7 +1966,7 @@
         <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1980,7 +1980,7 @@
         <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1994,7 +1994,7 @@
         <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2019,7 +2019,7 @@
         <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2033,7 +2033,7 @@
         <v>80</v>
       </c>
       <c r="D41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2047,7 +2047,7 @@
         <v>82</v>
       </c>
       <c r="D42" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2061,7 +2061,7 @@
         <v>84</v>
       </c>
       <c r="D43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2075,7 +2075,7 @@
         <v>86</v>
       </c>
       <c r="D44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2089,7 +2089,7 @@
         <v>88</v>
       </c>
       <c r="D45" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2103,7 +2103,7 @@
         <v>90</v>
       </c>
       <c r="D46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2117,7 +2117,7 @@
         <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2131,7 +2131,7 @@
         <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2145,7 +2145,7 @@
         <v>96</v>
       </c>
       <c r="D49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2159,7 +2159,7 @@
         <v>98</v>
       </c>
       <c r="D50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2173,7 +2173,7 @@
         <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2187,7 +2187,7 @@
         <v>102</v>
       </c>
       <c r="D52" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2201,7 +2201,7 @@
         <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2215,7 +2215,7 @@
         <v>107</v>
       </c>
       <c r="D54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2243,7 +2243,7 @@
         <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2257,7 +2257,7 @@
         <v>113</v>
       </c>
       <c r="D57" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2271,7 +2271,7 @@
         <v>116</v>
       </c>
       <c r="D58" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2285,7 +2285,7 @@
         <v>118</v>
       </c>
       <c r="D59" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2299,7 +2299,7 @@
         <v>38</v>
       </c>
       <c r="D60" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2313,7 +2313,7 @@
         <v>38</v>
       </c>
       <c r="D61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2327,7 +2327,7 @@
         <v>38</v>
       </c>
       <c r="D62" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2341,7 +2341,7 @@
         <v>38</v>
       </c>
       <c r="D63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2355,7 +2355,7 @@
         <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2369,7 +2369,7 @@
         <v>126</v>
       </c>
       <c r="D65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2383,7 +2383,7 @@
         <v>128</v>
       </c>
       <c r="D66" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2397,7 +2397,7 @@
         <v>38</v>
       </c>
       <c r="D67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2411,7 +2411,7 @@
         <v>38</v>
       </c>
       <c r="D68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2425,7 +2425,7 @@
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2439,7 +2439,7 @@
         <v>38</v>
       </c>
       <c r="D70" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2453,7 +2453,7 @@
         <v>134</v>
       </c>
       <c r="D71" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2467,7 +2467,7 @@
         <v>136</v>
       </c>
       <c r="D72" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2481,7 +2481,7 @@
         <v>38</v>
       </c>
       <c r="D73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2495,7 +2495,7 @@
         <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2509,7 +2509,7 @@
         <v>38</v>
       </c>
       <c r="D75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2523,7 +2523,7 @@
         <v>38</v>
       </c>
       <c r="D76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2537,7 +2537,7 @@
         <v>142</v>
       </c>
       <c r="D77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2551,7 +2551,7 @@
         <v>144</v>
       </c>
       <c r="D78" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2565,7 +2565,7 @@
         <v>38</v>
       </c>
       <c r="D79" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2579,7 +2579,7 @@
         <v>38</v>
       </c>
       <c r="D80" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2593,7 +2593,7 @@
         <v>38</v>
       </c>
       <c r="D81" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2607,7 +2607,7 @@
         <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2621,7 +2621,7 @@
         <v>150</v>
       </c>
       <c r="D83" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2635,7 +2635,7 @@
         <v>152</v>
       </c>
       <c r="D84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2649,7 +2649,7 @@
         <v>38</v>
       </c>
       <c r="D85" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2663,7 +2663,7 @@
         <v>38</v>
       </c>
       <c r="D86" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2677,7 +2677,7 @@
         <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2691,7 +2691,7 @@
         <v>38</v>
       </c>
       <c r="D88" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2705,7 +2705,7 @@
         <v>158</v>
       </c>
       <c r="D89" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2719,7 +2719,7 @@
         <v>160</v>
       </c>
       <c r="D90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2733,7 +2733,7 @@
         <v>38</v>
       </c>
       <c r="D91" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2747,7 +2747,7 @@
         <v>38</v>
       </c>
       <c r="D92" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2761,7 +2761,7 @@
         <v>38</v>
       </c>
       <c r="D93" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2775,7 +2775,7 @@
         <v>38</v>
       </c>
       <c r="D94" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2789,7 +2789,7 @@
         <v>166</v>
       </c>
       <c r="D95" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2803,7 +2803,7 @@
         <v>168</v>
       </c>
       <c r="D96" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2817,7 +2817,7 @@
         <v>170</v>
       </c>
       <c r="D97" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2831,7 +2831,7 @@
         <v>173</v>
       </c>
       <c r="D98" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2845,7 +2845,7 @@
         <v>175</v>
       </c>
       <c r="D99" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2859,7 +2859,7 @@
         <v>38</v>
       </c>
       <c r="D100" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2873,7 +2873,7 @@
         <v>38</v>
       </c>
       <c r="D101" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2887,7 +2887,7 @@
         <v>38</v>
       </c>
       <c r="D102" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2901,7 +2901,7 @@
         <v>38</v>
       </c>
       <c r="D103" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2915,7 +2915,7 @@
         <v>182</v>
       </c>
       <c r="D104" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2929,7 +2929,7 @@
         <v>184</v>
       </c>
       <c r="D105" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2943,7 +2943,7 @@
         <v>38</v>
       </c>
       <c r="D106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2957,7 +2957,7 @@
         <v>38</v>
       </c>
       <c r="D107" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2971,7 +2971,7 @@
         <v>38</v>
       </c>
       <c r="D108" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2985,7 +2985,7 @@
         <v>38</v>
       </c>
       <c r="D109" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2999,7 +2999,7 @@
         <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3013,7 +3013,7 @@
         <v>192</v>
       </c>
       <c r="D111" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3027,7 +3027,7 @@
         <v>38</v>
       </c>
       <c r="D112" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3041,7 +3041,7 @@
         <v>38</v>
       </c>
       <c r="D113" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3055,7 +3055,7 @@
         <v>38</v>
       </c>
       <c r="D114" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3069,7 +3069,7 @@
         <v>38</v>
       </c>
       <c r="D115" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3083,7 +3083,7 @@
         <v>198</v>
       </c>
       <c r="D116" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3097,7 +3097,7 @@
         <v>201</v>
       </c>
       <c r="D117" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3111,7 +3111,7 @@
         <v>203</v>
       </c>
       <c r="D118" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3125,7 +3125,7 @@
         <v>38</v>
       </c>
       <c r="D119" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3139,7 +3139,7 @@
         <v>38</v>
       </c>
       <c r="D120" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3153,7 +3153,7 @@
         <v>38</v>
       </c>
       <c r="D121" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3167,7 +3167,7 @@
         <v>38</v>
       </c>
       <c r="D122" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3181,7 +3181,7 @@
         <v>209</v>
       </c>
       <c r="D123" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3195,7 +3195,7 @@
         <v>211</v>
       </c>
       <c r="D124" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3209,7 +3209,7 @@
         <v>38</v>
       </c>
       <c r="D125" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3223,7 +3223,7 @@
         <v>38</v>
       </c>
       <c r="D126" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3237,7 +3237,7 @@
         <v>38</v>
       </c>
       <c r="D127" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3251,7 +3251,7 @@
         <v>38</v>
       </c>
       <c r="D128" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3265,7 +3265,7 @@
         <v>217</v>
       </c>
       <c r="D129" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3279,7 +3279,7 @@
         <v>219</v>
       </c>
       <c r="D130" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3293,7 +3293,7 @@
         <v>38</v>
       </c>
       <c r="D131" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3307,7 +3307,7 @@
         <v>38</v>
       </c>
       <c r="D132" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3321,7 +3321,7 @@
         <v>38</v>
       </c>
       <c r="D133" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3335,7 +3335,7 @@
         <v>38</v>
       </c>
       <c r="D134" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3349,7 +3349,7 @@
         <v>225</v>
       </c>
       <c r="D135" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3363,7 +3363,7 @@
         <v>227</v>
       </c>
       <c r="D136" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3377,7 +3377,7 @@
         <v>38</v>
       </c>
       <c r="D137" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3391,7 +3391,7 @@
         <v>38</v>
       </c>
       <c r="D138" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3405,7 +3405,7 @@
         <v>38</v>
       </c>
       <c r="D139" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3419,7 +3419,7 @@
         <v>38</v>
       </c>
       <c r="D140" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3433,7 +3433,7 @@
         <v>233</v>
       </c>
       <c r="D141" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3447,7 +3447,7 @@
         <v>235</v>
       </c>
       <c r="D142" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3461,7 +3461,7 @@
         <v>38</v>
       </c>
       <c r="D143" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3475,7 +3475,7 @@
         <v>38</v>
       </c>
       <c r="D144" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3489,7 +3489,7 @@
         <v>38</v>
       </c>
       <c r="D145" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3503,7 +3503,7 @@
         <v>38</v>
       </c>
       <c r="D146" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3517,7 +3517,7 @@
         <v>242</v>
       </c>
       <c r="D147" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3531,7 +3531,7 @@
         <v>244</v>
       </c>
       <c r="D148" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3545,7 +3545,7 @@
         <v>38</v>
       </c>
       <c r="D149" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3559,7 +3559,7 @@
         <v>38</v>
       </c>
       <c r="D150" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3573,7 +3573,7 @@
         <v>38</v>
       </c>
       <c r="D151" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3587,7 +3587,7 @@
         <v>38</v>
       </c>
       <c r="D152" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3601,7 +3601,7 @@
         <v>251</v>
       </c>
       <c r="D153" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3615,7 +3615,7 @@
         <v>253</v>
       </c>
       <c r="D154" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3629,7 +3629,7 @@
         <v>38</v>
       </c>
       <c r="D155" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3643,7 +3643,7 @@
         <v>38</v>
       </c>
       <c r="D156" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3657,7 +3657,7 @@
         <v>38</v>
       </c>
       <c r="D157" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3671,7 +3671,7 @@
         <v>38</v>
       </c>
       <c r="D158" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3685,7 +3685,7 @@
         <v>259</v>
       </c>
       <c r="D159" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3699,7 +3699,7 @@
         <v>261</v>
       </c>
       <c r="D160" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3713,7 +3713,7 @@
         <v>38</v>
       </c>
       <c r="D161" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3727,7 +3727,7 @@
         <v>38</v>
       </c>
       <c r="D162" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3741,7 +3741,7 @@
         <v>38</v>
       </c>
       <c r="D163" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3755,7 +3755,7 @@
         <v>38</v>
       </c>
       <c r="D164" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3769,7 +3769,7 @@
         <v>267</v>
       </c>
       <c r="D165" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3783,7 +3783,7 @@
         <v>269</v>
       </c>
       <c r="D166" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3797,7 +3797,7 @@
         <v>38</v>
       </c>
       <c r="D167" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3811,7 +3811,7 @@
         <v>38</v>
       </c>
       <c r="D168" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3825,7 +3825,7 @@
         <v>273</v>
       </c>
       <c r="D169" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3839,7 +3839,7 @@
         <v>276</v>
       </c>
       <c r="D170" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3853,7 +3853,7 @@
         <v>278</v>
       </c>
       <c r="D171" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3867,7 +3867,7 @@
         <v>38</v>
       </c>
       <c r="D172" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3881,7 +3881,7 @@
         <v>38</v>
       </c>
       <c r="D173" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3895,7 +3895,7 @@
         <v>38</v>
       </c>
       <c r="D174" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3909,7 +3909,7 @@
         <v>38</v>
       </c>
       <c r="D175" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3923,7 +3923,7 @@
         <v>284</v>
       </c>
       <c r="D176" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3937,7 +3937,7 @@
         <v>286</v>
       </c>
       <c r="D177" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3951,7 +3951,7 @@
         <v>38</v>
       </c>
       <c r="D178" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3965,7 +3965,7 @@
         <v>38</v>
       </c>
       <c r="D179" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3979,7 +3979,7 @@
         <v>38</v>
       </c>
       <c r="D180" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -3993,7 +3993,7 @@
         <v>38</v>
       </c>
       <c r="D181" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -4007,7 +4007,7 @@
         <v>292</v>
       </c>
       <c r="D182" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -4021,7 +4021,7 @@
         <v>294</v>
       </c>
       <c r="D183" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="14" x14ac:dyDescent="0.15">

</xml_diff>